<commit_message>
Commiting changes in Global laocal nav
</commit_message>
<xml_diff>
--- a/Mendix/input/data/Global_Vendor_Data.xlsx
+++ b/Mendix/input/data/Global_Vendor_Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SatishKumarSundaramo\git\Mendix_New\Mendix\input\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IBM_ADMIN\git\MIP\Mendix\input\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5487586C-7E25-4CD1-9174-2BF49FE6A54F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C9C62A-DCDC-4C86-8325-1BA84ECA3F07}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" xr2:uid="{92753D1E-95E7-49CB-AD96-B588CC3DB29F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9528" xr2:uid="{92753D1E-95E7-49CB-AD96-B588CC3DB29F}"/>
   </bookViews>
   <sheets>
     <sheet name="Y001" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="117">
   <si>
     <t>Fields</t>
   </si>
@@ -368,6 +368,15 @@
   </si>
   <si>
     <t>SG004OC</t>
+  </si>
+  <si>
+    <t>EN,English</t>
+  </si>
+  <si>
+    <t>Company Trading Partner</t>
+  </si>
+  <si>
+    <t>AE01</t>
   </si>
 </sst>
 </file>
@@ -870,66 +879,69 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B1D1E45-5652-489D-98CC-1DC9815FE9A3}">
-  <dimension ref="A1:BL6"/>
+  <dimension ref="A1:BM6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="AX1" workbookViewId="0">
+      <selection activeCell="BM3" sqref="BM3:BM6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="52.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.109375" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="19.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="19.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5546875" style="6" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.33203125" style="6" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="19" style="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="22.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.88671875" style="6" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="17" style="6" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.140625" style="6"/>
-    <col min="20" max="20" width="20.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="22.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="22.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="27.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="30.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="20.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="13.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="36.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="20.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="6.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="36.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="20.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="7.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="9.140625" style="4"/>
-    <col min="39" max="39" width="20.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="40" max="42" width="9.140625" style="4"/>
+    <col min="17" max="17" width="12.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.21875" style="6" customWidth="1"/>
+    <col min="19" max="19" width="13.88671875" style="6" customWidth="1"/>
+    <col min="20" max="20" width="20.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="20.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="22.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="22.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="27.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="30.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="20.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="36.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="20.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="6.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="36.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="20.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="7.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="9.109375" style="4"/>
+    <col min="39" max="39" width="20.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="40" max="42" width="9.109375" style="4"/>
     <col min="43" max="43" width="19" style="4" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="9.140625" style="4"/>
-    <col min="45" max="45" width="36.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="9.109375" style="4"/>
+    <col min="45" max="45" width="36.109375" style="4" bestFit="1" customWidth="1"/>
     <col min="46" max="46" width="33" style="4" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="36.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="31.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="36.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="31.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="24.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="14.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="53" max="16384" width="9.140625" style="4"/>
+    <col min="47" max="47" width="36.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="31.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="36.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="31.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="24.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="14.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="53" max="63" width="9.109375" style="4"/>
+    <col min="64" max="64" width="9.6640625" style="4" customWidth="1"/>
+    <col min="65" max="65" width="22.5546875" style="4" customWidth="1"/>
+    <col min="66" max="16384" width="9.109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:65" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1122,8 +1134,11 @@
       <c r="BL1" s="16" t="s">
         <v>89</v>
       </c>
+      <c r="BM1" s="8" t="s">
+        <v>115</v>
+      </c>
     </row>
-    <row r="2" spans="1:64" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:65" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -1314,8 +1329,11 @@
       <c r="BL2" s="17" t="s">
         <v>90</v>
       </c>
+      <c r="BM2" s="17" t="s">
+        <v>116</v>
+      </c>
     </row>
-    <row r="3" spans="1:64" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:65" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -1506,8 +1524,11 @@
       <c r="BL3" s="17" t="s">
         <v>90</v>
       </c>
+      <c r="BM3" s="17" t="s">
+        <v>116</v>
+      </c>
     </row>
-    <row r="4" spans="1:64" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:65" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -1698,8 +1719,11 @@
       <c r="BL4" s="17" t="s">
         <v>90</v>
       </c>
+      <c r="BM4" s="17" t="s">
+        <v>116</v>
+      </c>
     </row>
-    <row r="5" spans="1:64" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:65" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>74</v>
       </c>
@@ -1890,8 +1914,11 @@
       <c r="BL5" s="17" t="s">
         <v>90</v>
       </c>
+      <c r="BM5" s="17" t="s">
+        <v>116</v>
+      </c>
     </row>
-    <row r="6" spans="1:64" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:65" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>112</v>
       </c>
@@ -1940,7 +1967,7 @@
         <v>100</v>
       </c>
       <c r="R6" s="7" t="s">
-        <v>50</v>
+        <v>114</v>
       </c>
       <c r="S6" s="5" t="s">
         <v>107</v>
@@ -2079,6 +2106,9 @@
       </c>
       <c r="BL6" s="17" t="s">
         <v>90</v>
+      </c>
+      <c r="BM6" s="17" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Committing test plan excel sheet with test data
</commit_message>
<xml_diff>
--- a/Mendix/input/data/Global_Vendor_Data.xlsx
+++ b/Mendix/input/data/Global_Vendor_Data.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IBM_ADMIN\git\MIP\Mendix\input\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IBM_ADMIN\Git\New folder\MIP\Mendix\input\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C9C62A-DCDC-4C86-8325-1BA84ECA3F07}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9528" xr2:uid="{92753D1E-95E7-49CB-AD96-B588CC3DB29F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9528"/>
   </bookViews>
   <sheets>
     <sheet name="Y001" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -382,7 +381,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -878,11 +877,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B1D1E45-5652-489D-98CC-1DC9815FE9A3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BM6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AX1" workbookViewId="0">
-      <selection activeCell="BM3" sqref="BM3:BM6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1731,7 +1730,7 @@
         <v>73</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>7</v>
+        <v>75</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>41</v>
@@ -1926,7 +1925,7 @@
         <v>111</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>75</v>
+        <v>7</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>99</v>
@@ -2113,21 +2112,21 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="AT2" r:id="rId1" xr:uid="{303E161E-6DF5-4E52-BB98-200C2AB54574}"/>
-    <hyperlink ref="AV2" r:id="rId2" xr:uid="{327AA3EC-2BAF-4227-BC35-B19AB5CD03E9}"/>
-    <hyperlink ref="AX2" r:id="rId3" xr:uid="{71928824-78E3-40AE-8184-C6DFC10CA30F}"/>
-    <hyperlink ref="AT3" r:id="rId4" xr:uid="{86A0AC79-5308-48D6-9BC4-8FEDFEDA595D}"/>
-    <hyperlink ref="AV3" r:id="rId5" xr:uid="{80DE7D54-14CC-4E12-A223-CB6E32468345}"/>
-    <hyperlink ref="AX3" r:id="rId6" xr:uid="{2FC2D68D-0B9B-4705-BBE8-C65BC19DFBC3}"/>
-    <hyperlink ref="AT4" r:id="rId7" xr:uid="{96AE3302-B3F2-459A-B15A-E377BD23306B}"/>
-    <hyperlink ref="AV4" r:id="rId8" xr:uid="{DDDF9B4E-A389-46EE-8499-8801F1734766}"/>
-    <hyperlink ref="AX4" r:id="rId9" xr:uid="{9C75E0A7-8892-454E-9EDC-98F6B75BE028}"/>
-    <hyperlink ref="AT5" r:id="rId10" xr:uid="{CF721208-FD84-48B8-98FF-96ECEEEB6B32}"/>
-    <hyperlink ref="AV5" r:id="rId11" xr:uid="{77A5A758-1ACA-45A0-B214-C9B49D4F54F9}"/>
-    <hyperlink ref="AX5" r:id="rId12" xr:uid="{2120C1B1-F872-4A9B-9BA8-C1DF5510F8FF}"/>
-    <hyperlink ref="AT6" r:id="rId13" xr:uid="{86D9A581-0AF9-4255-94D3-BFCE24C41BA7}"/>
-    <hyperlink ref="AV6" r:id="rId14" xr:uid="{9E1AFF94-3F22-413D-80BE-8145035A0DB0}"/>
-    <hyperlink ref="AX6" r:id="rId15" xr:uid="{20D541CF-1D11-46B2-AD43-DEA896F8FDF3}"/>
+    <hyperlink ref="AT2" r:id="rId1"/>
+    <hyperlink ref="AV2" r:id="rId2"/>
+    <hyperlink ref="AX2" r:id="rId3"/>
+    <hyperlink ref="AT3" r:id="rId4"/>
+    <hyperlink ref="AV3" r:id="rId5"/>
+    <hyperlink ref="AX3" r:id="rId6"/>
+    <hyperlink ref="AT4" r:id="rId7"/>
+    <hyperlink ref="AV4" r:id="rId8"/>
+    <hyperlink ref="AX4" r:id="rId9"/>
+    <hyperlink ref="AT5" r:id="rId10"/>
+    <hyperlink ref="AV5" r:id="rId11"/>
+    <hyperlink ref="AX5" r:id="rId12"/>
+    <hyperlink ref="AT6" r:id="rId13"/>
+    <hyperlink ref="AV6" r:id="rId14"/>
+    <hyperlink ref="AX6" r:id="rId15"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId16"/>

</xml_diff>